<commit_message>
Added: New Result Updater
</commit_message>
<xml_diff>
--- a/Test_Cases.xlsx
+++ b/Test_Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\testing\bing-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FBACE0-6DB8-415B-A6A2-616B8DD5F7EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C4AD36-249F-4650-8D79-28E68D663588}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="4695" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Test Case</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>TC 2</t>
+  </si>
+  <si>
+    <t>Dhaka</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>TC 3</t>
   </si>
 </sst>
 </file>
@@ -357,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,6 +396,22 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done: Static landing page
</commit_message>
<xml_diff>
--- a/Test_Cases.xlsx
+++ b/Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\testing\bing-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8EC5DA-CEFA-4F0B-9EA3-067DCA87BA1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A784E3C-2936-4211-8638-3322582A1976}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,7 +366,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>